<commit_message>
Add Pendragon section; update Table 1
</commit_message>
<xml_diff>
--- a/tables/Pendragon.xlsx
+++ b/tables/Pendragon.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KAlstad\Documents\Github_C\e-deviceIEP\tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A3697A8D-AAF3-4167-BF66-53BE4EC3A33C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD2E9622-B568-4513-88C1-33968E9249DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-12465" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{E4A5BE10-DBB8-481B-874B-1BDF43DE8625}"/>
+    <workbookView xWindow="16335" yWindow="-16395" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{E4A5BE10-DBB8-481B-874B-1BDF43DE8625}"/>
   </bookViews>
   <sheets>
     <sheet name="Forms_Options" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="113">
   <si>
     <t>Feature</t>
   </si>
@@ -175,9 +175,6 @@
     <t>User Accessability</t>
   </si>
   <si>
-    <t>Flexibility to configure in a logical order for field entry (e.g., nested desgin)</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Audit trails </t>
     </r>
@@ -459,17 +456,184 @@
     <t>Price (Option 2)</t>
   </si>
   <si>
-    <t>Can provide tracking</t>
+    <t>Drop down option, radio buttons (selection list), look up list can reference another form.</t>
+  </si>
+  <si>
+    <t>Also, can get more sophisticated with scripting.  Logic of survey where subsequent question are based on the responses of earlier questions.</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Unless more complex forms required, and this would require Java scripting</t>
+  </si>
+  <si>
+    <t>Pendragon Server software can be either Cloud-based or 'On-premise'.</t>
+  </si>
+  <si>
+    <t>Default form is .csv</t>
+  </si>
+  <si>
+    <t>Not standard</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cloud upload is done manually as a separate step; separate mode from the Form/data entry mode.</t>
+  </si>
+  <si>
+    <t>Azure is FedRAMP certified; but Pendragon use is not certified</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cloud version -  Azure (central US); On-premise (users server)  </t>
+  </si>
+  <si>
+    <t>U.S.A.</t>
+  </si>
+  <si>
+    <t>Android systems provide more flexibility for customization (iOS requires certifications)</t>
+  </si>
+  <si>
+    <t>No drawing option integrated in Pendration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Photo integration supported for both OS </t>
+  </si>
+  <si>
+    <t>Actually only works in off line mode.  When the data transfer synch occurs, one is out of the Forms entry mode.</t>
+  </si>
+  <si>
+    <t>Only android feature can provide tracking.  Some trig functions available.  Theoretically could calculate distance using 'native' Pendragon scripting; but could also use Java scripting to develop a more advance calculation (e.g., survey distance)</t>
+  </si>
+  <si>
+    <t>Flexibility to configure in a logical order for field entry (e.g., nested design)</t>
+  </si>
+  <si>
+    <t>Azure</t>
+  </si>
+  <si>
+    <t>No further information</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Pendragon</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Forms</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> is a software as a service (SaaS) cloud application paid via monthly subscription based on the number of reserved users. However, an On Premise version is also offered for organizations who cannot or do not want to use a cloud-based solution.</t>
+    </r>
+  </si>
+  <si>
+    <t>Price (Option 3)</t>
+  </si>
+  <si>
+    <t>Cloud Standard: 10-24 Users; Storage 5GB</t>
+  </si>
+  <si>
+    <t>Cloud Professional: 25-99 Users; Storage 10GB</t>
+  </si>
+  <si>
+    <t>Cloud Essentials: 2-9 Users; Storage
+1 GB</t>
+  </si>
+  <si>
+    <t>$40/mo/2 users</t>
+  </si>
+  <si>
+    <t>$260/mo/14 users</t>
+  </si>
+  <si>
+    <t>$560/mo/28 users</t>
+  </si>
+  <si>
+    <t>Price (Option 5)</t>
+  </si>
+  <si>
+    <t>https://pendragonforms.com/pendragon_pricing_on_premise.html</t>
+  </si>
+  <si>
+    <t>On-premise option allows organizations with restrictive IT policies or requirements for tighter integration to install on their local servers.</t>
+  </si>
+  <si>
+    <t>Pendragon "QuickStart" Our support specialists will guide you through the initial steps of converting your paper forms to digital forms so that you can begin collecting data in minutes.</t>
+  </si>
+  <si>
+    <t>Not provided</t>
+  </si>
+  <si>
+    <t>Dan Phillips (Pendragon) suggests that Pendragon falls into the middle of the array of e-device software options: between the very simple, quick menu driven and completely customized form developed from scratch using base coding languages.</t>
+  </si>
+  <si>
+    <t>No information</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Three different types of users.  User can only get in from the interface on the device and cannot design or change the data collection form;  Designer can design forms but cannot control users;  Admin and do all of it.  Completed forms can be assigned to groups and users can be added to have access to these forms.</t>
+  </si>
+  <si>
+    <t>Voice to text can be used for text fields</t>
+  </si>
+  <si>
+    <t>Yes/No</t>
+  </si>
+  <si>
+    <t>Custom API connections are available which could support user-developed version control routines.</t>
+  </si>
+  <si>
+    <t>Pendragon saves the form in a relational database on MySQLdatabase server.  Further processes would be needed to download and transfer these relational tables to the user/project database. Custom API connections are available which could support integration with user/project database.</t>
+  </si>
+  <si>
+    <t>Maybe</t>
+  </si>
+  <si>
+    <t>Establishing communication to external sensors would require Pendragon tech time/fees; apparently they have done this a couple of times.</t>
+  </si>
+  <si>
+    <t>Web-based only</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -570,6 +734,39 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF5E5E5E"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color rgb="FF5E5E5E"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -592,7 +789,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -651,6 +848,31 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="6" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -974,8 +1196,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FEDC525-B77D-4397-8B91-1C5526620A5B}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="105" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView topLeftCell="A15" zoomScale="105" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -996,19 +1218,19 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="111" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>31</v>
       </c>
@@ -1016,10 +1238,10 @@
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1027,7 +1249,13 @@
         <v>31</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1037,6 +1265,12 @@
       <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="C4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>71</v>
+      </c>
       <c r="F4"/>
     </row>
     <row r="5" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1044,7 +1278,10 @@
         <v>31</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1054,6 +1291,9 @@
       <c r="B6" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="C6" s="1" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="7" spans="1:6" ht="84.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -1062,9 +1302,15 @@
       <c r="B7" t="s">
         <v>9</v>
       </c>
+      <c r="C7" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>103</v>
+      </c>
       <c r="E7" s="13"/>
     </row>
-    <row r="8" spans="1:6" ht="72" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="72" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>31</v>
       </c>
@@ -1072,12 +1318,18 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="51" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="102.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1087,6 +1339,12 @@
       <c r="B10" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="C10" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>73</v>
+      </c>
       <c r="F10" s="15"/>
     </row>
     <row r="11" spans="1:6" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1096,21 +1354,33 @@
       <c r="B11" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="C11" s="1" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="12" spans="1:6" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>31</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="78" customHeight="1" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>35</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>33</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D13" s="24" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1120,6 +1390,9 @@
       <c r="B14" t="s">
         <v>8</v>
       </c>
+      <c r="C14" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="D14" s="2"/>
     </row>
     <row r="15" spans="1:6" ht="69" customHeight="1" x14ac:dyDescent="0.25">
@@ -1129,6 +1402,12 @@
       <c r="B15" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="C15" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="E15" s="14"/>
     </row>
     <row r="16" spans="1:6" ht="87" customHeight="1" x14ac:dyDescent="0.25">
@@ -1138,13 +1417,25 @@
       <c r="B16" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="89.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>36</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>34</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>
@@ -1182,72 +1473,97 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="119.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D2" s="2"/>
+        <v>61</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="E2" s="7"/>
     </row>
     <row r="3" spans="1:7" ht="132.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="C3" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>109</v>
+      </c>
       <c r="E3" s="5"/>
     </row>
-    <row r="4" spans="1:7" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="C5" s="1" t="s">
+        <v>104</v>
+      </c>
       <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:7" s="4" customFormat="1" ht="129" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>13</v>
       </c>
+      <c r="C6" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>75</v>
+      </c>
       <c r="E6" s="10"/>
       <c r="F6" s="5"/>
     </row>
     <row r="7" spans="1:7" ht="78" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="4"/>
+      <c r="C7" s="4" t="s">
+        <v>65</v>
+      </c>
       <c r="D7" s="4"/>
       <c r="E7" s="20"/>
       <c r="F7" s="5"/>
@@ -1255,27 +1571,44 @@
     </row>
     <row r="8" spans="1:7" ht="104.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="5"/>
+      <c r="C8" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="9" spans="1:7" ht="118.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="C9" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="10" spans="1:7" ht="109.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -1288,14 +1621,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DF5D6FA-27AF-4377-9AE3-FE0575D1CE52}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35.140625" customWidth="1"/>
-    <col min="2" max="2" width="26.7109375" customWidth="1"/>
+    <col min="2" max="2" width="26.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="18.7109375" customWidth="1"/>
     <col min="4" max="4" width="39.140625" customWidth="1"/>
     <col min="5" max="5" width="34.140625" customWidth="1"/>
@@ -1310,88 +1643,112 @@
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" t="s">
         <v>60</v>
-      </c>
-      <c r="F1" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="4" customFormat="1" ht="132" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>20</v>
       </c>
+      <c r="C2" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="3" spans="1:6" s="4" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C3" s="16"/>
+      <c r="C3" s="4" t="s">
+        <v>65</v>
+      </c>
       <c r="D3" s="16"/>
       <c r="F3" s="7"/>
     </row>
     <row r="4" spans="1:6" ht="54.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>46</v>
-      </c>
-      <c r="B4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>22</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>65</v>
       </c>
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:6" ht="86.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>46</v>
-      </c>
-      <c r="B5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+        <v>45</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>82</v>
+      </c>
       <c r="E5" s="17"/>
       <c r="F5" s="18"/>
     </row>
     <row r="6" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C6" s="1"/>
+        <v>46</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>65</v>
+      </c>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
     <row r="7" spans="1:6" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>65</v>
       </c>
       <c r="E7" s="4"/>
     </row>
     <row r="8" spans="1:6" ht="93" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+      <c r="C8" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>111</v>
+      </c>
       <c r="E8" s="1"/>
     </row>
   </sheetData>
@@ -1404,8 +1761,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6FF90FC-7D54-4396-BEBF-836B30C262EA}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:D8"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1419,16 +1776,16 @@
   <sheetData>
     <row r="1" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>60</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1439,12 +1796,21 @@
     </row>
     <row r="3" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="70.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="11" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="44.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="11" t="s">
-        <v>53</v>
+      <c r="B4" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" s="29" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="48" customHeight="1" x14ac:dyDescent="0.25">
@@ -1454,17 +1820,32 @@
     </row>
     <row r="6" spans="1:4" ht="54" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="47.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="104.25" customHeight="1" x14ac:dyDescent="0.3">
+        <v>54</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>24</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -1478,14 +1859,14 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:E6"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="49.140625" customWidth="1"/>
     <col min="2" max="2" width="38.5703125" customWidth="1"/>
-    <col min="3" max="3" width="40.85546875" customWidth="1"/>
+    <col min="3" max="3" width="40.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="18.140625" customWidth="1"/>
     <col min="5" max="5" width="36.28515625" customWidth="1"/>
   </cols>
@@ -1495,54 +1876,70 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" t="s">
         <v>60</v>
-      </c>
-      <c r="E1" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="9"/>
+      <c r="B2" s="9" t="s">
+        <v>80</v>
+      </c>
       <c r="C2" s="9"/>
       <c r="D2" s="4"/>
     </row>
-    <row r="3" spans="1:5" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="9"/>
+      <c r="B3" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C3" s="23" t="s">
+        <v>89</v>
+      </c>
       <c r="D3" s="7"/>
     </row>
     <row r="4" spans="1:5" ht="108" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="4"/>
+      <c r="B4" s="4" t="s">
+        <v>79</v>
+      </c>
       <c r="C4" s="9"/>
     </row>
     <row r="5" spans="1:5" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="9"/>
+      <c r="B5" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="6" spans="1:5" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
+      <c r="B6" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>88</v>
+      </c>
       <c r="D6" s="9"/>
     </row>
   </sheetData>
@@ -1553,17 +1950,17 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41DAF0C1-5840-4498-93BE-7596EB0B3995}">
-  <dimension ref="A1:G8"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="27.85546875" customWidth="1"/>
-    <col min="2" max="2" width="36.28515625" customWidth="1"/>
-    <col min="3" max="3" width="28.5703125" customWidth="1"/>
+    <col min="2" max="2" width="36.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="28.5703125" style="21" customWidth="1"/>
     <col min="4" max="4" width="24.5703125" customWidth="1"/>
     <col min="5" max="5" width="46.140625" customWidth="1"/>
   </cols>
@@ -1576,61 +1973,108 @@
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>60</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>61</v>
       </c>
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
     </row>
-    <row r="2" spans="1:7" ht="85.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="1"/>
+        <v>48</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>94</v>
+      </c>
       <c r="D2" s="4"/>
       <c r="E2" s="1"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
     </row>
-    <row r="3" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
+        <v>69</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>95</v>
+      </c>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="1:7" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
+        <v>90</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>96</v>
+      </c>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="4"/>
       <c r="G4" s="4"/>
     </row>
-    <row r="5" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B5" s="4"/>
+        <v>97</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C5" s="25">
+        <v>3950</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+    </row>
+    <row r="6" spans="1:7" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="26"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+    </row>
+    <row r="7" spans="1:7" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="28" t="s">
+        <v>100</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E8" s="19"/>
+      <c r="B8" s="27"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E10" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>